<commit_message>
Documentatie aangepast en callHandler geimplementeerd
</commit_message>
<xml_diff>
--- a/doc/Andalusier todo documentatie/ToDo technisch.xlsx
+++ b/doc/Andalusier todo documentatie/ToDo technisch.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BamPistache\Desktop\Andalusier todo documentatie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\andalusier\htdocs\andalusier\doc\Andalusier todo documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Prio</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Algemeen</t>
   </si>
   <si>
-    <t>Implementeer PHAJAX</t>
-  </si>
-  <si>
     <t>Betere documentatie bij stukken code</t>
   </si>
   <si>
@@ -102,13 +99,19 @@
   </si>
   <si>
     <t>Mappen kunnen verwijderen als er andere bestanden inzitten</t>
+  </si>
+  <si>
+    <t>Implementeer PHAJAX (callHandler)</t>
+  </si>
+  <si>
+    <t>Error systeem inbouwen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -124,8 +127,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -150,6 +160,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -163,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -175,9 +191,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -193,9 +210,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -233,7 +250,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -268,6 +285,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -303,9 +337,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -455,15 +506,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -478,142 +529,148 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="B3" s="7"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="6"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="5"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="6"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="6"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="5"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="B25" s="5"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="5"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B25" s="1"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="5"/>
+      <c r="B32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>